<commit_message>
añadiendo la eliminacion de los registros con datos incorrectos en el csv.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -474,13 +474,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>185080</v>
+        <v>177271</v>
       </c>
       <c r="D2" t="n">
-        <v>1899541.760000044</v>
+        <v>1897495.680000036</v>
       </c>
       <c r="E2" t="n">
-        <v>117768</v>
+        <v>112301</v>
       </c>
     </row>
     <row r="3">
@@ -495,13 +495,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>63469</v>
+        <v>60379</v>
       </c>
       <c r="D3" t="n">
-        <v>635403.2300000053</v>
+        <v>634690.0400000043</v>
       </c>
       <c r="E3" t="n">
-        <v>39963</v>
+        <v>37880</v>
       </c>
     </row>
     <row r="4">
@@ -516,13 +516,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>156621</v>
+        <v>149863</v>
       </c>
       <c r="D4" t="n">
-        <v>1631009.440000045</v>
+        <v>1628945.43000004</v>
       </c>
       <c r="E4" t="n">
-        <v>100800</v>
+        <v>96089</v>
       </c>
     </row>
     <row r="5">
@@ -537,13 +537,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>63710</v>
+        <v>60561</v>
       </c>
       <c r="D5" t="n">
-        <v>633585.9000000054</v>
+        <v>632690.6500000041</v>
       </c>
       <c r="E5" t="n">
-        <v>40030</v>
+        <v>37912</v>
       </c>
     </row>
     <row r="6">
@@ -558,13 +558,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>63592</v>
+        <v>60448</v>
       </c>
       <c r="D6" t="n">
-        <v>661851.7000000031</v>
+        <v>660756.8200000003</v>
       </c>
       <c r="E6" t="n">
-        <v>41484</v>
+        <v>39258</v>
       </c>
     </row>
     <row r="7">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>27093</v>
+        <v>25681</v>
       </c>
       <c r="D7" t="n">
-        <v>276021.1400000007</v>
+        <v>275461.1300000007</v>
       </c>
       <c r="E7" t="n">
-        <v>17478</v>
+        <v>16500</v>
       </c>
     </row>
   </sheetData>
@@ -646,13 +646,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6952623</v>
+        <v>6897913</v>
       </c>
       <c r="D2" t="n">
-        <v>11393206.87999875</v>
+        <v>11369332.68999879</v>
       </c>
       <c r="E2" t="n">
-        <v>4663589</v>
+        <v>4618013</v>
       </c>
     </row>
     <row r="3">
@@ -667,13 +667,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2323876</v>
+        <v>2308458</v>
       </c>
       <c r="D3" t="n">
-        <v>3650607.769999944</v>
+        <v>3642218.109999947</v>
       </c>
       <c r="E3" t="n">
-        <v>1463042</v>
+        <v>1451048</v>
       </c>
     </row>
     <row r="4">
@@ -688,13 +688,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6381098</v>
+        <v>6335233</v>
       </c>
       <c r="D4" t="n">
-        <v>10446535.26999961</v>
+        <v>10423945.63999971</v>
       </c>
       <c r="E4" t="n">
-        <v>4329379</v>
+        <v>4291341</v>
       </c>
     </row>
     <row r="5">
@@ -709,13 +709,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2725750</v>
+        <v>2706845</v>
       </c>
       <c r="D5" t="n">
-        <v>4276544.209999817</v>
+        <v>4264982.189999899</v>
       </c>
       <c r="E5" t="n">
-        <v>1728079</v>
+        <v>1713625</v>
       </c>
     </row>
     <row r="6">
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3138554</v>
+        <v>3112053</v>
       </c>
       <c r="D6" t="n">
-        <v>5375047.199999955</v>
+        <v>5360842.019999959</v>
       </c>
       <c r="E6" t="n">
-        <v>2175646</v>
+        <v>2153295</v>
       </c>
     </row>
     <row r="7">
@@ -751,13 +751,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1093646</v>
+        <v>1085008</v>
       </c>
       <c r="D7" t="n">
-        <v>1862253.499999984</v>
+        <v>1856013.899999982</v>
       </c>
       <c r="E7" t="n">
-        <v>710739</v>
+        <v>703879</v>
       </c>
     </row>
   </sheetData>
@@ -818,13 +818,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>59428</v>
+        <v>38527</v>
       </c>
       <c r="D2" t="n">
-        <v>991468.6599999944</v>
+        <v>1004739.729999992</v>
       </c>
       <c r="E2" t="n">
-        <v>94946</v>
+        <v>77782</v>
       </c>
     </row>
     <row r="3">
@@ -839,13 +839,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>22247</v>
+        <v>13398</v>
       </c>
       <c r="D3" t="n">
-        <v>194317.1999999998</v>
+        <v>196196.8399999999</v>
       </c>
       <c r="E3" t="n">
-        <v>25788</v>
+        <v>19272</v>
       </c>
     </row>
     <row r="4">
@@ -860,13 +860,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>51328</v>
+        <v>33635</v>
       </c>
       <c r="D4" t="n">
-        <v>848587.9899999888</v>
+        <v>844561.2199999882</v>
       </c>
       <c r="E4" t="n">
-        <v>73742</v>
+        <v>60647</v>
       </c>
     </row>
     <row r="5">
@@ -881,13 +881,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>25021</v>
+        <v>14653</v>
       </c>
       <c r="D5" t="n">
-        <v>208464.3699999988</v>
+        <v>206438.879999999</v>
       </c>
       <c r="E5" t="n">
-        <v>27354</v>
+        <v>20087</v>
       </c>
     </row>
     <row r="6">
@@ -902,13 +902,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23484</v>
+        <v>14896</v>
       </c>
       <c r="D6" t="n">
-        <v>1048625.939999988</v>
+        <v>1046400.299999988</v>
       </c>
       <c r="E6" t="n">
-        <v>46848</v>
+        <v>40429</v>
       </c>
     </row>
     <row r="7">
@@ -923,13 +923,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>11130</v>
+        <v>6690</v>
       </c>
       <c r="D7" t="n">
-        <v>148069.7299999999</v>
+        <v>146991.6700000001</v>
       </c>
       <c r="E7" t="n">
-        <v>14704</v>
+        <v>11522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>